<commit_message>
Fixed one unified language + README formatting
</commit_message>
<xml_diff>
--- a/3/hundmänniskor.xlsx
+++ b/3/hundmänniskor.xlsx
@@ -424,32 +424,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Namn</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Ålder</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Epost</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Mobil</t>
+          <t>Mobile</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Djurnamn</t>
+          <t>Pet Name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Ras</t>
+          <t>Breed</t>
         </is>
       </c>
     </row>
@@ -1992,7 +1992,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Medelålder:</t>
+          <t>Average age:</t>
         </is>
       </c>
       <c r="B57">
@@ -2003,7 +2003,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Medianålder:</t>
+          <t>Median age:</t>
         </is>
       </c>
       <c r="B58">
@@ -2014,7 +2014,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Yngst:</t>
+          <t>Youngest:</t>
         </is>
       </c>
       <c r="B59">
@@ -2025,7 +2025,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Äldst:</t>
+          <t>Oldest:</t>
         </is>
       </c>
       <c r="B60">

</xml_diff>